<commit_message>
Update documents - Wu Zheming 2024/05/15
</commit_message>
<xml_diff>
--- a/Professional_Study/Software_Engineering_MAI/Course_Project/Documents/Backlog_TimeEstimation.xlsx
+++ b/Professional_Study/Software_Engineering_MAI/Course_Project/Documents/Backlog_TimeEstimation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\学习相关\研二课程\Software Engineering\Course_Project\Submit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\学习相关\研二课程\Software Engineering\Course_Project\Submit\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3516F1FD-2468-4219-8701-FE8BB20A21B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEBB54B-F8E2-45DE-9892-C5A5A36EBBBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Task</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -43,15 +43,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Monitoring computer program running background</t>
-  </si>
-  <si>
-    <t>Record the running time of each application</t>
-  </si>
-  <si>
-    <t>Identify which applications are games</t>
-  </si>
-  <si>
     <t>Monitor</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -66,13 +57,6 @@
     <t>Remind children when approaching the time limit</t>
   </si>
   <si>
-    <t>Automatically lock the computer when reach game time limit</t>
-  </si>
-  <si>
-    <t>Parents can remotely unlock computers through mobile phones</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Draw statistics graph of game time</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -94,6 +78,34 @@
   </si>
   <si>
     <t>Man/Day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Monitoring computer program running process</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Identify which application processes are games</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Automatically interrupt the game process when reach game time limit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parents can remotely interrupt the game process through mobile phones</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Record the running time of each game application process</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cloud(Telegram)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Transfer commands and data through the Cloud (e.g. Telegram)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -419,25 +431,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="54.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.19921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
@@ -456,35 +469,35 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -492,10 +505,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -503,13 +516,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -517,35 +530,52 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E10">
         <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>0.5</v>
+      </c>
+      <c r="E11">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>